<commit_message>
Push to pull on new PC
</commit_message>
<xml_diff>
--- a/docs/Process.xlsx
+++ b/docs/Process.xlsx
@@ -535,7 +535,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,6 +566,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -821,9 +827,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -887,28 +890,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1520,7 +1526,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E18" sqref="E18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,10 +1731,10 @@
       <c r="B11" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="33"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
       <c r="H11" s="22"/>
@@ -1747,10 +1753,10 @@
       <c r="B12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="33"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>
@@ -1769,10 +1775,10 @@
       <c r="B13" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="33"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="20"/>
       <c r="G13" s="21"/>
       <c r="H13" s="22"/>
@@ -1791,10 +1797,10 @@
       <c r="B14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="33"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="20"/>
       <c r="G14" s="21"/>
       <c r="H14" s="22"/>
@@ -1830,13 +1836,13 @@
       <c r="A16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
       <c r="K16" s="20"/>
       <c r="L16" s="21"/>
       <c r="M16" s="23"/>
@@ -1850,154 +1856,154 @@
       <c r="B17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="37" t="s">
+      <c r="D17" s="33"/>
+      <c r="E17" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="37" t="s">
+      <c r="D18" s="33"/>
+      <c r="E18" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="37" t="s">
+      <c r="G18" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="38"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="37" t="s">
+      <c r="D19" s="33"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="I19" s="37" t="s">
+      <c r="I19" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="37" t="s">
+      <c r="J19" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="38"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="37" t="s">
+      <c r="D20" s="33"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="K20" s="37" t="s">
+      <c r="K20" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="L20" s="37" t="s">
+      <c r="L20" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="41"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="20"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="44" t="s">
+      <c r="E21" s="38"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="N21" s="37" t="s">
+      <c r="N21" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="38"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="37" t="s">
+      <c r="D22" s="47"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="P22" s="37" t="s">
+      <c r="P22" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="Q22" s="37" t="s">
+      <c r="Q22" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="R22" s="37" t="s">
+      <c r="R22" s="36" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2006,22 +2012,22 @@
         <v>49</v>
       </c>
       <c r="D23" s="20"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="37" t="s">
+      <c r="E23" s="38"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="R23" s="37" t="s">
+      <c r="R23" s="36" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2029,59 +2035,59 @@
       <c r="B24" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="52"/>
-      <c r="M25" s="53"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="51"/>
+      <c r="M25" s="52"/>
     </row>
     <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="54" t="s">
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="H26" s="55"/>
+      <c r="H26" s="57"/>
       <c r="I26" s="14"/>
-      <c r="L26" s="54" t="s">
+      <c r="L26" s="55" t="s">
         <v>72</v>
       </c>
       <c r="M26" s="56"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G27" s="57" t="s">
+      <c r="G27" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="H27" s="57"/>
-      <c r="L27" s="58" t="s">
+      <c r="H27" s="58"/>
+      <c r="L27" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="M27" s="58"/>
-      <c r="R27" s="59" t="s">
+      <c r="M27" s="59"/>
+      <c r="R27" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L28" s="60"/>
       <c r="M28" s="60"/>
-      <c r="R28" s="61" t="s">
+      <c r="R28" s="54" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Login API is now online
Move successful logins to Home Page
First steps in Create Account Page
</commit_message>
<xml_diff>
--- a/docs/Process.xlsx
+++ b/docs/Process.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ibrahem Mansour\DopaChat\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746DE0F2-E415-4512-84C1-86289DED7A84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6D8553-9363-43F1-91D7-5F5C6D00011B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -900,6 +900,9 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -917,9 +920,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1530,7 +1530,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,7 +1861,7 @@
         <v>11</v>
       </c>
       <c r="D17" s="33"/>
-      <c r="E17" s="62" t="s">
+      <c r="E17" s="56" t="s">
         <v>63</v>
       </c>
       <c r="F17" s="37"/>
@@ -1883,13 +1883,13 @@
         <v>44</v>
       </c>
       <c r="D18" s="33"/>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="56" t="s">
         <v>20</v>
       </c>
       <c r="H18" s="39"/>
@@ -2065,32 +2065,32 @@
     <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
-      <c r="G26" s="56" t="s">
+      <c r="G26" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="H26" s="58"/>
+      <c r="H26" s="59"/>
       <c r="I26" s="14"/>
-      <c r="L26" s="56" t="s">
+      <c r="L26" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="M26" s="57"/>
+      <c r="M26" s="58"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G27" s="59" t="s">
+      <c r="G27" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="H27" s="59"/>
-      <c r="L27" s="60" t="s">
+      <c r="H27" s="60"/>
+      <c r="L27" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="M27" s="60"/>
+      <c r="M27" s="61"/>
       <c r="R27" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="L28" s="61"/>
-      <c r="M28" s="61"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
       <c r="R28" s="54" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Work on Create Account Page:
	getCities
	Countries
</commit_message>
<xml_diff>
--- a/docs/Process.xlsx
+++ b/docs/Process.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ibrahem Mansour\DopaChat\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6D8553-9363-43F1-91D7-5F5C6D00011B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FDC99C-D98F-4CE1-B9C4-537F369D6C73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
     <sheet name="Timetable" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -891,16 +891,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1530,7 +1530,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="I19" sqref="I19:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,7 +1735,7 @@
       <c r="B11" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="55" t="s">
+      <c r="D11" s="53" t="s">
         <v>62</v>
       </c>
       <c r="E11" s="32"/>
@@ -1757,7 +1757,7 @@
       <c r="B12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="53" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="32"/>
@@ -1779,7 +1779,7 @@
       <c r="B13" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="53" t="s">
         <v>62</v>
       </c>
       <c r="E13" s="32"/>
@@ -1801,7 +1801,7 @@
       <c r="B14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="55" t="s">
+      <c r="D14" s="53" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="32"/>
@@ -1861,7 +1861,7 @@
         <v>11</v>
       </c>
       <c r="D17" s="33"/>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="54" t="s">
         <v>63</v>
       </c>
       <c r="F17" s="37"/>
@@ -1883,13 +1883,13 @@
         <v>44</v>
       </c>
       <c r="D18" s="33"/>
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="56" t="s">
+      <c r="G18" s="54" t="s">
         <v>20</v>
       </c>
       <c r="H18" s="39"/>
@@ -2084,14 +2084,14 @@
         <v>52</v>
       </c>
       <c r="M27" s="61"/>
-      <c r="R27" s="53" t="s">
+      <c r="R27" s="55" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L28" s="62"/>
       <c r="M28" s="62"/>
-      <c r="R28" s="54" t="s">
+      <c r="R28" s="56" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added SearchPeople and Results page
</commit_message>
<xml_diff>
--- a/docs/Process.xlsx
+++ b/docs/Process.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ibrahem Mansour\DopaChat\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FDC99C-D98F-4CE1-B9C4-537F369D6C73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8756CA57-3A62-4366-987F-83442096501B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -861,9 +861,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -920,6 +917,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1529,9 +1529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:J19"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1735,7 +1733,7 @@
       <c r="B11" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="52" t="s">
         <v>62</v>
       </c>
       <c r="E11" s="32"/>
@@ -1757,7 +1755,7 @@
       <c r="B12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="52" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="32"/>
@@ -1779,7 +1777,7 @@
       <c r="B13" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="52" t="s">
         <v>62</v>
       </c>
       <c r="E13" s="32"/>
@@ -1801,7 +1799,7 @@
       <c r="B14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="52" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="32"/>
@@ -1861,7 +1859,7 @@
         <v>11</v>
       </c>
       <c r="D17" s="33"/>
-      <c r="E17" s="54" t="s">
+      <c r="E17" s="53" t="s">
         <v>63</v>
       </c>
       <c r="F17" s="37"/>
@@ -1883,13 +1881,13 @@
         <v>44</v>
       </c>
       <c r="D18" s="33"/>
-      <c r="E18" s="54" t="s">
+      <c r="E18" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="F18" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="54" t="s">
+      <c r="G18" s="53" t="s">
         <v>20</v>
       </c>
       <c r="H18" s="39"/>
@@ -1911,16 +1909,16 @@
       <c r="D19" s="33"/>
       <c r="E19" s="41"/>
       <c r="F19" s="42"/>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="I19" s="36" t="s">
+      <c r="I19" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="36" t="s">
+      <c r="J19" s="53" t="s">
         <v>20</v>
       </c>
       <c r="K19" s="37"/>
@@ -1940,16 +1938,16 @@
       <c r="D20" s="33"/>
       <c r="E20" s="41"/>
       <c r="F20" s="42"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="45"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="44"/>
       <c r="I20" s="37"/>
-      <c r="J20" s="36" t="s">
+      <c r="J20" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="L20" s="36" t="s">
+      <c r="L20" s="53" t="s">
         <v>20</v>
       </c>
       <c r="M20" s="40"/>
@@ -1967,15 +1965,15 @@
       <c r="E21" s="38"/>
       <c r="F21" s="42"/>
       <c r="G21" s="41"/>
-      <c r="H21" s="46"/>
+      <c r="H21" s="45"/>
       <c r="I21" s="37"/>
       <c r="J21" s="37"/>
       <c r="K21" s="37"/>
       <c r="L21" s="38"/>
-      <c r="M21" s="43" t="s">
+      <c r="M21" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="N21" s="36" t="s">
+      <c r="N21" s="53" t="s">
         <v>20</v>
       </c>
       <c r="O21" s="37"/>
@@ -1987,11 +1985,11 @@
       <c r="B22" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="47"/>
+      <c r="D22" s="46"/>
       <c r="E22" s="41"/>
       <c r="F22" s="42"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="46"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="45"/>
       <c r="I22" s="37"/>
       <c r="J22" s="37"/>
       <c r="K22" s="37"/>
@@ -2019,7 +2017,7 @@
       <c r="E23" s="38"/>
       <c r="F23" s="42"/>
       <c r="G23" s="41"/>
-      <c r="H23" s="46"/>
+      <c r="H23" s="45"/>
       <c r="I23" s="42"/>
       <c r="J23" s="37"/>
       <c r="K23" s="37"/>
@@ -2039,14 +2037,14 @@
       <c r="B24" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="49"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="37"/>
       <c r="F24" s="42"/>
       <c r="G24" s="41"/>
-      <c r="H24" s="46"/>
+      <c r="H24" s="45"/>
       <c r="I24" s="42"/>
       <c r="J24" s="42"/>
-      <c r="K24" s="50"/>
+      <c r="K24" s="49"/>
       <c r="L24" s="38"/>
       <c r="M24" s="40"/>
       <c r="N24" s="37"/>
@@ -2056,42 +2054,42 @@
       <c r="R24" s="37"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="51"/>
-      <c r="M25" s="52"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="50"/>
+      <c r="M25" s="51"/>
     </row>
     <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="57" t="s">
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="H26" s="59"/>
+      <c r="H26" s="58"/>
       <c r="I26" s="14"/>
-      <c r="L26" s="57" t="s">
+      <c r="L26" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="M26" s="58"/>
+      <c r="M26" s="57"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G27" s="60" t="s">
+      <c r="G27" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="H27" s="60"/>
-      <c r="L27" s="61" t="s">
+      <c r="H27" s="59"/>
+      <c r="L27" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="M27" s="61"/>
-      <c r="R27" s="55" t="s">
+      <c r="M27" s="60"/>
+      <c r="R27" s="54" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="L28" s="62"/>
-      <c r="M28" s="62"/>
-      <c r="R28" s="56" t="s">
+      <c r="L28" s="61"/>
+      <c r="M28" s="61"/>
+      <c r="R28" s="55" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>